<commit_message>
feat: add multi rules tables
</commit_message>
<xml_diff>
--- a/test/rules.xlsx
+++ b/test/rules.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\agarimojs\rules\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0644CC8-A590-47B0-9C2A-4F15785E7A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0193D619-32DA-4F9E-B71A-1018D22FD1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Types" sheetId="2" r:id="rId1"/>
     <sheet name="Spreadsheet" sheetId="3" r:id="rId2"/>
     <sheet name="Methods" sheetId="4" r:id="rId3"/>
     <sheet name="Rules" sheetId="1" r:id="rId4"/>
+    <sheet name="Multi" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>C1</t>
   </si>
@@ -402,6 +403,65 @@
   </si>
   <si>
     <t>return str.split(/\r?\n/);</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>[25..66]</t>
+  </si>
+  <si>
+    <t>[33..74]</t>
+  </si>
+  <si>
+    <t>&lt;50</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Multi String </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Multi1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(String measure1, Integer measure2)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1031,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD389B69-8614-4E76-8361-6D85067E4D81}">
   <dimension ref="B3:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1264,7 +1324,7 @@
   <dimension ref="B3:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="B3" sqref="B3:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1575,4 +1635,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8095BA3E-D432-4761-AA62-5C5BEE424EA7}">
+  <dimension ref="C5:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
+      <c r="D6" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+      <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C13" s="1"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D6:H6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add constants table, better context
</commit_message>
<xml_diff>
--- a/test/rules.xlsx
+++ b/test/rules.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\agarimojs\rules\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0193D619-32DA-4F9E-B71A-1018D22FD1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A28CD8-F681-4BBF-A16D-6CCF2153DDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Types" sheetId="2" r:id="rId1"/>
-    <sheet name="Spreadsheet" sheetId="3" r:id="rId2"/>
-    <sheet name="Methods" sheetId="4" r:id="rId3"/>
-    <sheet name="Rules" sheetId="1" r:id="rId4"/>
-    <sheet name="Multi" sheetId="5" r:id="rId5"/>
+    <sheet name="Constants" sheetId="6" r:id="rId2"/>
+    <sheet name="Spreadsheet" sheetId="3" r:id="rId3"/>
+    <sheet name="Methods" sheetId="4" r:id="rId4"/>
+    <sheet name="Rules" sheetId="1" r:id="rId5"/>
+    <sheet name="Multi" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
   <si>
     <t>C1</t>
   </si>
@@ -463,12 +464,33 @@
       <t>(String measure1, Integer measure2)</t>
     </r>
   </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>defaultName</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>defaultState</t>
+  </si>
+  <si>
+    <t>defaultMeasure</t>
+  </si>
+  <si>
+    <t>=defaultName</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -579,6 +601,14 @@
       <u/>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -720,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -773,6 +803,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1092,7 +1131,7 @@
   <dimension ref="B3:F10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B3" sqref="B3:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,6 +1228,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CC1FE8-192D-402A-B395-D56D5F119349}">
+  <dimension ref="C4:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
+      <c r="D6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="8">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="8">
+        <v>12.7</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECDD7FF-DB46-4C9B-98BE-39C7D1D5CE07}">
   <dimension ref="B3:E10"/>
   <sheetViews>
@@ -1280,7 +1404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F048D32-3FDE-431D-99B7-5583694854BD}">
   <dimension ref="C3:C9"/>
   <sheetViews>
@@ -1319,12 +1443,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C957CE-038E-47C5-A6BF-BB08E128B598}">
   <dimension ref="B3:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1441,7 +1565,7 @@
       <c r="C10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="26" t="s">
         <v>32</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1637,15 +1761,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8095BA3E-D432-4761-AA62-5C5BEE424EA7}">
   <dimension ref="C5:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
@@ -1764,11 +1891,11 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="5"/>
       <c r="E13" s="4" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
feat: add check table to check return values from tables
</commit_message>
<xml_diff>
--- a/test/rules.xlsx
+++ b/test/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\agarimo\rules\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA80048D-F1C6-48B1-9971-67AD8488ABBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C9D8F2-762F-4597-B835-2ED663372EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="5" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Types" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Spreadsheet" sheetId="3" r:id="rId3"/>
     <sheet name="Methods" sheetId="4" r:id="rId4"/>
     <sheet name="Rules" sheetId="1" r:id="rId5"/>
-    <sheet name="Multi" sheetId="5" r:id="rId6"/>
-    <sheet name="Tests" sheetId="7" r:id="rId7"/>
+    <sheet name="Checks" sheetId="8" r:id="rId6"/>
+    <sheet name="Multi" sheetId="5" r:id="rId7"/>
+    <sheet name="Tests" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="122">
   <si>
     <t>C1</t>
   </si>
@@ -676,6 +677,15 @@
       </rPr>
       <t>(String measure1, Integer measure2)</t>
     </r>
+  </si>
+  <si>
+    <t>Check RuleCheck</t>
+  </si>
+  <si>
+    <t>Rule1</t>
+  </si>
+  <si>
+    <t>Rule2</t>
   </si>
 </sst>
 </file>
@@ -856,7 +866,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -938,11 +948,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1006,6 +1025,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1640,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C957CE-038E-47C5-A6BF-BB08E128B598}">
   <dimension ref="B3:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -2084,6 +2106,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A49B299-C683-42B7-A0F6-533548777A21}">
+  <dimension ref="C6:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="1"/>
+      <c r="D7" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8095BA3E-D432-4761-AA62-5C5BEE424EA7}">
   <dimension ref="C5:I14"/>
   <sheetViews>
@@ -2247,12 +2318,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111D7AF6-AE25-4398-94FD-9436EF2AA7D8}">
   <dimension ref="C9:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: add RET types code and codes
</commit_message>
<xml_diff>
--- a/test/rules.xlsx
+++ b/test/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\agarimo\rules\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C9D8F2-762F-4597-B835-2ED663372EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6026F0A8-44C5-459F-856A-16ED652E4000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="5" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="4" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Types" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="131">
   <si>
     <t>C1</t>
   </si>
@@ -686,6 +686,38 @@
   </si>
   <si>
     <t>Rule2</t>
+  </si>
+  <si>
+    <t>Rules String Rule4(String measure3, String measure1, Integer measure2)</t>
+  </si>
+  <si>
+    <t>codes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoA1 
+ NoA2
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NoB1
+</t>
+  </si>
+  <si>
+    <t>NoA3,NoA4
+NoA5</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Rules String Rule5(String measure3, String measure1, Integer measure2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NoA1 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    NoA3,NoA4NoA5    </t>
   </si>
 </sst>
 </file>
@@ -1002,6 +1034,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1025,9 +1060,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1349,30 +1381,30 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1383,7 +1415,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
         <v>3</v>
@@ -1394,7 +1426,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="6" t="s">
         <v>17</v>
@@ -1405,7 +1437,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
         <v>3</v>
@@ -1416,7 +1448,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="6" t="s">
         <v>3</v>
@@ -1427,7 +1459,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1450,30 +1482,30 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.69140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C5" s="1"/>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
         <v>3</v>
@@ -1486,7 +1518,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C7" s="1"/>
       <c r="D7" s="6" t="s">
         <v>74</v>
@@ -1499,7 +1531,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C8" s="1"/>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -1512,7 +1544,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1535,27 +1567,27 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="46.77734375" customWidth="1"/>
-    <col min="4" max="4" width="83.88671875" customWidth="1"/>
+    <col min="3" max="3" width="46.765625" customWidth="1"/>
+    <col min="4" max="4" width="83.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B3" s="1"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="24"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
         <v>20</v>
@@ -1565,7 +1597,7 @@
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="12" t="s">
         <v>50</v>
@@ -1575,7 +1607,7 @@
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="12" t="s">
         <v>52</v>
@@ -1585,7 +1617,7 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="12" t="s">
         <v>54</v>
@@ -1595,7 +1627,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="12" t="s">
         <v>55</v>
@@ -1605,7 +1637,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1627,27 +1659,27 @@
       <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:3" ht="16.3" x14ac:dyDescent="0.5">
       <c r="C3" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C4" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="3:3" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:3" ht="16.3" x14ac:dyDescent="0.5">
       <c r="C8" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.4">
       <c r="C9" s="17" t="s">
         <v>23</v>
       </c>
@@ -1660,24 +1692,24 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C957CE-038E-47C5-A6BF-BB08E128B598}">
-  <dimension ref="B3:J40"/>
+  <dimension ref="B3:J64"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.53515625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.765625" customWidth="1"/>
+    <col min="6" max="6" width="17.84375" customWidth="1"/>
+    <col min="7" max="7" width="14.765625" customWidth="1"/>
+    <col min="8" max="8" width="16.53515625" customWidth="1"/>
+    <col min="9" max="9" width="26.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1686,18 +1718,18 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -1711,7 +1743,7 @@
       <c r="F5" s="2"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>24</v>
@@ -1723,7 +1755,7 @@
       <c r="F6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
@@ -1737,7 +1769,7 @@
       <c r="F7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
         <v>24</v>
@@ -1756,7 +1788,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:8" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="25.75" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="5" t="s">
         <v>29</v>
@@ -1775,7 +1807,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:8" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" ht="25.75" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="5" t="s">
         <v>30</v>
@@ -1794,7 +1826,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1803,7 +1835,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1813,19 +1845,19 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C21" s="1"/>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C22" s="1"/>
       <c r="D22" s="2" t="s">
         <v>0</v>
@@ -1841,7 +1873,7 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C23" s="1"/>
       <c r="D23" s="2" t="s">
         <v>37</v>
@@ -1857,7 +1889,7 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C24" s="1"/>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -1873,7 +1905,7 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C25" s="1"/>
       <c r="D25" s="3" t="s">
         <v>18</v>
@@ -1895,9 +1927,9 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="3:10" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
       <c r="C26" s="1"/>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1917,9 +1949,9 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="3:10" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
       <c r="C27" s="1"/>
-      <c r="D27" s="27"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="5" t="s">
         <v>30</v>
       </c>
@@ -1937,7 +1969,7 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="3:10" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
       <c r="C28" s="1"/>
       <c r="D28" s="15" t="s">
         <v>5</v>
@@ -1957,7 +1989,7 @@
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1967,7 +1999,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1976,18 +2008,18 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C33" s="1"/>
-      <c r="D33" s="25" t="s">
+      <c r="D33" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C34" s="1"/>
       <c r="D34" s="2" t="s">
         <v>0</v>
@@ -2001,7 +2033,7 @@
       <c r="G34" s="2"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C35" s="1"/>
       <c r="D35" s="2" t="s">
         <v>24</v>
@@ -2013,7 +2045,7 @@
       <c r="G35" s="2"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C36" s="1"/>
       <c r="D36" s="2" t="s">
         <v>3</v>
@@ -2027,7 +2059,7 @@
       <c r="G36" s="2"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C37" s="1"/>
       <c r="D37" s="3" t="s">
         <v>24</v>
@@ -2046,7 +2078,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C38" s="1"/>
       <c r="D38" s="5" t="s">
         <v>29</v>
@@ -2065,7 +2097,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C39" s="1"/>
       <c r="D39" s="5" t="s">
         <v>30</v>
@@ -2084,7 +2116,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2093,12 +2125,320 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C44" s="1"/>
+      <c r="D44" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C45" s="1"/>
+      <c r="D45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C46" s="1"/>
+      <c r="D46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C47" s="1"/>
+      <c r="D47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C48" s="1"/>
+      <c r="D48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
+      <c r="C49" s="1"/>
+      <c r="D49" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
+      <c r="C50" s="1"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
+      <c r="C51" s="1"/>
+      <c r="D51" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="15"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C56" s="1"/>
+      <c r="D56" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="26"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="1"/>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C57" s="1"/>
+      <c r="D57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J57" s="1"/>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C58" s="1"/>
+      <c r="D58" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="2"/>
+      <c r="J58" s="1"/>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C59" s="1"/>
+      <c r="D59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="J59" s="1"/>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C60" s="1"/>
+      <c r="D60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60" s="1"/>
+    </row>
+    <row r="61" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
+      <c r="C61" s="1"/>
+      <c r="D61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="1"/>
+    </row>
+    <row r="62" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
+      <c r="C62" s="1"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="1"/>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C63" s="1"/>
+      <c r="D63" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="15"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="1"/>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D56:I56"/>
+    <mergeCell ref="D61:D62"/>
     <mergeCell ref="D21:I21"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D44:I44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2109,42 +2449,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A49B299-C683-42B7-A0F6-533548777A21}">
   <dimension ref="C6:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="4" max="4" width="17.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C7" s="1"/>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="20" t="s">
         <v>119</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C8" s="1"/>
       <c r="D8" s="4" t="s">
         <v>120</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C9" s="1"/>
       <c r="D9" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2162,12 +2502,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2176,18 +2516,18 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C6" s="1"/>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
         <v>0</v>
@@ -2201,7 +2541,7 @@
       <c r="G7" s="2"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
         <v>24</v>
@@ -2213,7 +2553,7 @@
       <c r="G8" s="2"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -2227,7 +2567,7 @@
       <c r="G9" s="2"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C10" s="1"/>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -2246,7 +2586,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C11" s="1"/>
       <c r="D11" s="5" t="s">
         <v>29</v>
@@ -2265,7 +2605,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C12" s="1"/>
       <c r="D12" s="5" t="s">
         <v>30</v>
@@ -2284,7 +2624,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="3:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C13" s="1"/>
       <c r="D13" s="5"/>
       <c r="E13" s="4" t="s">
@@ -2301,7 +2641,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2326,32 +2666,32 @@
       <selection activeCell="C9" sqref="C9:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="5" max="5" width="15.109375" customWidth="1"/>
-    <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="12" max="12" width="19.77734375" customWidth="1"/>
+    <col min="5" max="5" width="15.07421875" customWidth="1"/>
+    <col min="6" max="6" width="23.07421875" customWidth="1"/>
+    <col min="9" max="9" width="17.53515625" customWidth="1"/>
+    <col min="12" max="12" width="19.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C10" s="1"/>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
       <c r="G10" s="1"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C11" s="1"/>
       <c r="D11" s="3" t="s">
         <v>25</v>
@@ -2364,7 +2704,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C12" s="1"/>
       <c r="D12" s="5">
         <v>10</v>
@@ -2377,7 +2717,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C13" s="1"/>
       <c r="D13" s="5">
         <v>27</v>
@@ -2390,7 +2730,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C14" s="1"/>
       <c r="D14" s="5">
         <v>51</v>
@@ -2403,7 +2743,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C15" s="1"/>
       <c r="D15" s="5">
         <v>75</v>
@@ -2416,7 +2756,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.4">
       <c r="C16" s="1"/>
       <c r="D16" s="5">
         <v>12</v>
@@ -2429,7 +2769,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C17" s="1"/>
       <c r="D17" s="5">
         <v>30</v>
@@ -2442,7 +2782,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C18" s="1"/>
       <c r="D18" s="5">
         <v>50</v>
@@ -2455,7 +2795,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C19" s="1"/>
       <c r="D19" s="5">
         <v>76</v>
@@ -2468,30 +2808,30 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C23" s="1"/>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C24" s="1"/>
       <c r="D24" s="3" t="s">
         <v>24</v>
@@ -2504,7 +2844,7 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C25" s="1"/>
       <c r="D25" s="5" t="s">
         <v>29</v>
@@ -2517,7 +2857,7 @@
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C26" s="1"/>
       <c r="D26" s="5" t="s">
         <v>29</v>
@@ -2530,7 +2870,7 @@
       </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C27" s="1"/>
       <c r="D27" s="5" t="s">
         <v>29</v>
@@ -2543,7 +2883,7 @@
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C28" s="1"/>
       <c r="D28" s="5" t="s">
         <v>29</v>
@@ -2556,7 +2896,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C29" s="1"/>
       <c r="D29" s="5" t="s">
         <v>30</v>
@@ -2569,7 +2909,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C30" s="1"/>
       <c r="D30" s="5" t="s">
         <v>30</v>
@@ -2582,7 +2922,7 @@
       </c>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C31" s="1"/>
       <c r="D31" s="5" t="s">
         <v>30</v>
@@ -2595,7 +2935,7 @@
       </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C32" s="1"/>
       <c r="D32" s="5" t="s">
         <v>30</v>
@@ -2608,30 +2948,30 @@
       </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C37" s="1"/>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C38" s="1"/>
       <c r="D38" s="3" t="s">
         <v>24</v>
@@ -2644,7 +2984,7 @@
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C39" s="1"/>
       <c r="D39" s="5" t="s">
         <v>29</v>
@@ -2657,7 +2997,7 @@
       </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C40" s="1"/>
       <c r="D40" s="5" t="s">
         <v>30</v>
@@ -2670,7 +3010,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C41" s="1"/>
       <c r="D41" s="5" t="s">
         <v>29</v>
@@ -2683,7 +3023,7 @@
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C42" s="1"/>
       <c r="D42" s="5" t="s">
         <v>30</v>
@@ -2696,7 +3036,7 @@
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="3:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C43" s="1"/>
       <c r="D43" s="5" t="s">
         <v>29</v>
@@ -2709,7 +3049,7 @@
       </c>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C44" s="1"/>
       <c r="D44" s="5" t="s">
         <v>30</v>
@@ -2722,7 +3062,7 @@
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C45" s="1"/>
       <c r="D45" s="5" t="s">
         <v>29</v>
@@ -2735,7 +3075,7 @@
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C46" s="1"/>
       <c r="D46" s="5" t="s">
         <v>30</v>
@@ -2748,7 +3088,7 @@
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C47" s="1"/>
       <c r="D47" s="5" t="s">
         <v>29</v>
@@ -2761,7 +3101,7 @@
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.4">
       <c r="C48" s="1"/>
       <c r="D48" s="5" t="s">
         <v>30</v>
@@ -2774,7 +3114,7 @@
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C49" s="1"/>
       <c r="D49" s="5" t="s">
         <v>29</v>
@@ -2787,7 +3127,7 @@
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C50" s="1"/>
       <c r="D50" s="5" t="s">
         <v>30</v>
@@ -2800,7 +3140,7 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C51" s="1"/>
       <c r="D51" s="5" t="s">
         <v>93</v>
@@ -2813,14 +3153,14 @@
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="56" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2833,22 +3173,22 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C57" s="1"/>
-      <c r="D57" s="25" t="s">
+      <c r="D57" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
-      <c r="L57" s="25"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="26"/>
+      <c r="L57" s="26"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C58" s="1"/>
       <c r="D58" s="3" t="s">
         <v>15</v>
@@ -2879,7 +3219,7 @@
       </c>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="3:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C59" s="1"/>
       <c r="D59" s="5" t="s">
         <v>108</v>
@@ -2910,7 +3250,7 @@
       </c>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:13" x14ac:dyDescent="0.4">
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>

</xml_diff>

<commit_message>
feat: checks matrix flat values should go through toValue
</commit_message>
<xml_diff>
--- a/test/rules.xlsx
+++ b/test/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\agarimo\rules\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6026F0A8-44C5-459F-856A-16ED652E4000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B0323C-3BFA-4526-A1D6-9FD00AF25E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="4" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="7" xr2:uid="{F97B6F4B-53D9-4DB4-8257-AA2F9CB2A1CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Types" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="139">
   <si>
     <t>C1</t>
   </si>
@@ -717,7 +717,57 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">    NoA3,NoA4NoA5    </t>
+    <t>NoA1,NoA2</t>
+  </si>
+  <si>
+    <t>NoA3,NoA4,NoA5</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Rule4 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rule4Test</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test Rule5 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rule5Test</t>
+    </r>
+  </si>
+  <si>
+    <t>NoA1</t>
+  </si>
+  <si>
+    <t>Rule4</t>
+  </si>
+  <si>
+    <t>Rule5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    NoA3  </t>
+  </si>
+  <si>
+    <t>NoA3</t>
   </si>
 </sst>
 </file>
@@ -1052,14 +1102,14 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1381,19 +1431,19 @@
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="21" t="s">
         <v>13</v>
@@ -1404,7 +1454,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="6" t="s">
         <v>3</v>
@@ -1415,7 +1465,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="6" t="s">
         <v>3</v>
@@ -1426,7 +1476,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="6" t="s">
         <v>17</v>
@@ -1437,7 +1487,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="6" t="s">
         <v>3</v>
@@ -1448,7 +1498,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="6" t="s">
         <v>3</v>
@@ -1459,7 +1509,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1482,19 +1532,19 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="23" t="s">
         <v>71</v>
@@ -1505,7 +1555,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
       <c r="D6" s="6" t="s">
         <v>3</v>
@@ -1518,7 +1568,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="6" t="s">
         <v>74</v>
@@ -1531,7 +1581,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="6" t="s">
         <v>17</v>
@@ -1544,7 +1594,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1567,19 +1617,19 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="46.765625" customWidth="1"/>
-    <col min="4" max="4" width="83.84375" customWidth="1"/>
+    <col min="3" max="3" width="46.77734375" customWidth="1"/>
+    <col min="4" max="4" width="83.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="25" t="s">
         <v>19</v>
@@ -1587,7 +1637,7 @@
       <c r="D4" s="25"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="10" t="s">
         <v>20</v>
@@ -1597,7 +1647,7 @@
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="12" t="s">
         <v>50</v>
@@ -1607,7 +1657,7 @@
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="12" t="s">
         <v>52</v>
@@ -1617,7 +1667,7 @@
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="12" t="s">
         <v>54</v>
@@ -1627,7 +1677,7 @@
       </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="12" t="s">
         <v>55</v>
@@ -1637,7 +1687,7 @@
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1659,27 +1709,27 @@
       <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:3" ht="16.3" x14ac:dyDescent="0.5">
+    <row r="3" spans="3:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="C3" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C4" s="17" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="3:3" ht="16.3" x14ac:dyDescent="0.5">
+    <row r="8" spans="3:3" ht="16.2" x14ac:dyDescent="0.35">
       <c r="C8" s="14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C9" s="17" t="s">
         <v>23</v>
       </c>
@@ -1694,22 +1744,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C957CE-038E-47C5-A6BF-BB08E128B598}">
   <dimension ref="B3:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.53515625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15.765625" customWidth="1"/>
-    <col min="6" max="6" width="17.84375" customWidth="1"/>
-    <col min="7" max="7" width="14.765625" customWidth="1"/>
-    <col min="8" max="8" width="16.53515625" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1718,18 +1768,18 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>0</v>
@@ -1743,7 +1793,7 @@
       <c r="F5" s="2"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>24</v>
@@ -1755,7 +1805,7 @@
       <c r="F6" s="2"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
@@ -1769,7 +1819,7 @@
       <c r="F7" s="2"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="3" t="s">
         <v>24</v>
@@ -1788,7 +1838,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="2:8" ht="25.75" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="5" t="s">
         <v>29</v>
@@ -1807,7 +1857,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:8" ht="25.75" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="5" t="s">
         <v>30</v>
@@ -1826,7 +1876,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1835,7 +1885,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1845,19 +1895,19 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="2" t="s">
         <v>0</v>
@@ -1873,7 +1923,7 @@
       </c>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="2" t="s">
         <v>37</v>
@@ -1889,7 +1939,7 @@
       </c>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="2" t="s">
         <v>3</v>
@@ -1905,7 +1955,7 @@
       </c>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="3" t="s">
         <v>18</v>
@@ -1927,9 +1977,9 @@
       </c>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
+    <row r="26" spans="3:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1949,9 +1999,9 @@
       </c>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
+    <row r="27" spans="3:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
-      <c r="D27" s="28"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="5" t="s">
         <v>30</v>
       </c>
@@ -1969,7 +2019,7 @@
       </c>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
+    <row r="28" spans="3:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="15" t="s">
         <v>5</v>
@@ -1989,7 +2039,7 @@
       </c>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1999,7 +2049,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2008,18 +2058,18 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="28"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="2" t="s">
         <v>0</v>
@@ -2033,7 +2083,7 @@
       <c r="G34" s="2"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="2" t="s">
         <v>24</v>
@@ -2045,7 +2095,7 @@
       <c r="G35" s="2"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="2" t="s">
         <v>3</v>
@@ -2059,7 +2109,7 @@
       <c r="G36" s="2"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="3" t="s">
         <v>24</v>
@@ -2078,7 +2128,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="5" t="s">
         <v>29</v>
@@ -2097,7 +2147,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="5" t="s">
         <v>30</v>
@@ -2116,7 +2166,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2125,7 +2175,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2135,19 +2185,19 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
-      <c r="D44" s="26" t="s">
+      <c r="D44" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="28"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="28"/>
+      <c r="I44" s="28"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
       <c r="D45" s="2" t="s">
         <v>0</v>
@@ -2163,7 +2213,7 @@
       </c>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
       <c r="D46" s="2" t="s">
         <v>37</v>
@@ -2177,7 +2227,7 @@
       <c r="G46" s="2"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="2" t="s">
         <v>3</v>
@@ -2193,7 +2243,7 @@
       </c>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="3" t="s">
         <v>18</v>
@@ -2215,9 +2265,9 @@
       </c>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
+    <row r="49" spans="3:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
-      <c r="D49" s="27" t="s">
+      <c r="D49" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E49" s="5" t="s">
@@ -2237,9 +2287,9 @@
       </c>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="3:10" ht="38.6" x14ac:dyDescent="0.4">
+    <row r="50" spans="3:10" ht="41.4" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
-      <c r="D50" s="28"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="5" t="s">
         <v>30</v>
       </c>
@@ -2257,7 +2307,7 @@
       </c>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
+    <row r="51" spans="3:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="15" t="s">
         <v>5</v>
@@ -2275,7 +2325,7 @@
       </c>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2285,7 +2335,7 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -2295,19 +2345,19 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C56" s="1"/>
-      <c r="D56" s="26" t="s">
+      <c r="D56" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
-      <c r="I56" s="26"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28"/>
+      <c r="G56" s="28"/>
+      <c r="H56" s="28"/>
+      <c r="I56" s="28"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C57" s="1"/>
       <c r="D57" s="2" t="s">
         <v>0</v>
@@ -2323,7 +2373,7 @@
       </c>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="58" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C58" s="1"/>
       <c r="D58" s="2" t="s">
         <v>37</v>
@@ -2337,7 +2387,7 @@
       <c r="G58" s="2"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="59" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C59" s="1"/>
       <c r="D59" s="2" t="s">
         <v>3</v>
@@ -2353,7 +2403,7 @@
       </c>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="60" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C60" s="1"/>
       <c r="D60" s="3" t="s">
         <v>18</v>
@@ -2375,9 +2425,9 @@
       </c>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
+    <row r="61" spans="3:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C61" s="1"/>
-      <c r="D61" s="27" t="s">
+      <c r="D61" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E61" s="5" t="s">
@@ -2387,15 +2437,15 @@
         <v>129</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="3:10" ht="25.75" x14ac:dyDescent="0.4">
+    <row r="62" spans="3:10" ht="27.6" x14ac:dyDescent="0.3">
       <c r="C62" s="1"/>
-      <c r="D62" s="28"/>
+      <c r="D62" s="27"/>
       <c r="E62" s="5" t="s">
         <v>30</v>
       </c>
@@ -2407,7 +2457,7 @@
       <c r="I62" s="4"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="63" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C63" s="1"/>
       <c r="D63" s="15" t="s">
         <v>5</v>
@@ -2419,7 +2469,7 @@
       <c r="I63" s="4"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="64" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -2447,47 +2497,61 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A49B299-C683-42B7-A0F6-533548777A21}">
-  <dimension ref="C6:E10"/>
+  <dimension ref="C6:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.07421875" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="20" t="s">
         <v>119</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="4" t="s">
         <v>120</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="4" t="s">
         <v>121</v>
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2502,12 +2566,12 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="15.53515625" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2516,18 +2580,18 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C6" s="1"/>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
         <v>0</v>
@@ -2541,7 +2605,7 @@
       <c r="G7" s="2"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
         <v>24</v>
@@ -2553,7 +2617,7 @@
       <c r="G8" s="2"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -2567,7 +2631,7 @@
       <c r="G9" s="2"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
       <c r="D10" s="3" t="s">
         <v>24</v>
@@ -2586,7 +2650,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="5" t="s">
         <v>29</v>
@@ -2605,7 +2669,7 @@
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="5" t="s">
         <v>30</v>
@@ -2624,7 +2688,7 @@
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="5"/>
       <c r="E13" s="4" t="s">
@@ -2641,7 +2705,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -2660,38 +2724,38 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{111D7AF6-AE25-4398-94FD-9436EF2AA7D8}">
-  <dimension ref="C9:M60"/>
+  <dimension ref="C9:M75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:G20"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="15.07421875" customWidth="1"/>
-    <col min="6" max="6" width="23.07421875" customWidth="1"/>
-    <col min="9" max="9" width="17.53515625" customWidth="1"/>
-    <col min="12" max="12" width="19.765625" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" customWidth="1"/>
+    <col min="6" max="7" width="23.109375" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="1"/>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="1"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="1"/>
       <c r="D11" s="3" t="s">
         <v>25</v>
@@ -2704,7 +2768,7 @@
       </c>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="5">
         <v>10</v>
@@ -2717,7 +2781,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="1"/>
       <c r="D13" s="5">
         <v>27</v>
@@ -2730,7 +2794,7 @@
       </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="5">
         <v>51</v>
@@ -2743,7 +2807,7 @@
       </c>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="5">
         <v>75</v>
@@ -2756,7 +2820,7 @@
       </c>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="5">
         <v>12</v>
@@ -2769,7 +2833,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="5">
         <v>30</v>
@@ -2782,7 +2846,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="5">
         <v>50</v>
@@ -2795,7 +2859,7 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="5">
         <v>76</v>
@@ -2808,30 +2872,30 @@
       </c>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="3" t="s">
         <v>24</v>
@@ -2844,7 +2908,7 @@
       </c>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="D25" s="5" t="s">
         <v>29</v>
@@ -2857,7 +2921,7 @@
       </c>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="5" t="s">
         <v>29</v>
@@ -2870,7 +2934,7 @@
       </c>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="5" t="s">
         <v>29</v>
@@ -2883,7 +2947,7 @@
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="5" t="s">
         <v>29</v>
@@ -2896,7 +2960,7 @@
       </c>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="5" t="s">
         <v>30</v>
@@ -2909,7 +2973,7 @@
       </c>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C30" s="1"/>
       <c r="D30" s="5" t="s">
         <v>30</v>
@@ -2922,7 +2986,7 @@
       </c>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="5" t="s">
         <v>30</v>
@@ -2935,7 +2999,7 @@
       </c>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="5" t="s">
         <v>30</v>
@@ -2948,30 +3012,30 @@
       </c>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
-      <c r="D37" s="26" t="s">
+      <c r="D37" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="3" t="s">
         <v>24</v>
@@ -2984,7 +3048,7 @@
       </c>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="5" t="s">
         <v>29</v>
@@ -2997,7 +3061,7 @@
       </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C40" s="1"/>
       <c r="D40" s="5" t="s">
         <v>30</v>
@@ -3010,7 +3074,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C41" s="1"/>
       <c r="D41" s="5" t="s">
         <v>29</v>
@@ -3023,7 +3087,7 @@
       </c>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C42" s="1"/>
       <c r="D42" s="5" t="s">
         <v>30</v>
@@ -3036,7 +3100,7 @@
       </c>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="3:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="3:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C43" s="1"/>
       <c r="D43" s="5" t="s">
         <v>29</v>
@@ -3049,7 +3113,7 @@
       </c>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C44" s="1"/>
       <c r="D44" s="5" t="s">
         <v>30</v>
@@ -3062,7 +3126,7 @@
       </c>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C45" s="1"/>
       <c r="D45" s="5" t="s">
         <v>29</v>
@@ -3075,7 +3139,7 @@
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C46" s="1"/>
       <c r="D46" s="5" t="s">
         <v>30</v>
@@ -3088,7 +3152,7 @@
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C47" s="1"/>
       <c r="D47" s="5" t="s">
         <v>29</v>
@@ -3101,7 +3165,7 @@
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.4">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C48" s="1"/>
       <c r="D48" s="5" t="s">
         <v>30</v>
@@ -3114,7 +3178,7 @@
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="49" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C49" s="1"/>
       <c r="D49" s="5" t="s">
         <v>29</v>
@@ -3127,7 +3191,7 @@
       </c>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="50" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C50" s="1"/>
       <c r="D50" s="5" t="s">
         <v>30</v>
@@ -3140,7 +3204,7 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="51" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C51" s="1"/>
       <c r="D51" s="5" t="s">
         <v>93</v>
@@ -3153,14 +3217,14 @@
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="52" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="56" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="56" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -3173,22 +3237,22 @@
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="57" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C57" s="1"/>
-      <c r="D57" s="26" t="s">
+      <c r="D57" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="E57" s="26"/>
-      <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="26"/>
-      <c r="K57" s="26"/>
-      <c r="L57" s="26"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
+      <c r="L57" s="28"/>
       <c r="M57" s="1"/>
     </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="58" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C58" s="1"/>
       <c r="D58" s="3" t="s">
         <v>15</v>
@@ -3219,7 +3283,7 @@
       </c>
       <c r="M58" s="1"/>
     </row>
-    <row r="59" spans="3:13" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="3:13" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C59" s="1"/>
       <c r="D59" s="5" t="s">
         <v>108</v>
@@ -3250,7 +3314,7 @@
       </c>
       <c r="M59" s="1"/>
     </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.4">
+    <row r="60" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -3263,8 +3327,158 @@
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
+    <row r="63" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+    </row>
+    <row r="64" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C64" s="1"/>
+      <c r="D64" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="1"/>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C65" s="1"/>
+      <c r="D65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C66" s="1"/>
+      <c r="D66" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E66" s="5">
+        <v>10</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="3:8" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="1"/>
+      <c r="D67" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E67" s="5">
+        <v>27</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C71" s="1"/>
+      <c r="D71" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C72" s="1"/>
+      <c r="D72" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C73" s="1"/>
+      <c r="D73" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E73" s="5">
+        <v>10</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H73" s="1"/>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C74" s="1"/>
+      <c r="D74" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E74" s="5">
+        <v>27</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D64:G64"/>
     <mergeCell ref="D10:F10"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D37:F37"/>

</xml_diff>